<commit_message>
create power threshold front
</commit_message>
<xml_diff>
--- a/rawdata/shotlist_Aug9.xlsx
+++ b/rawdata/shotlist_Aug9.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Repositories\MScThesis\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F390C659-6652-4D8B-8218-778706194D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5BF328-554D-4C67-A7DD-195BF991CE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1335" windowWidth="31275" windowHeight="13770" xr2:uid="{52462B7A-835B-47F1-ADEF-6175C6EA22AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{52462B7A-835B-47F1-ADEF-6175C6EA22AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Shotlist V2" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Information" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="105">
   <si>
     <t>Shot #</t>
   </si>
@@ -391,6 +392,12 @@
   </si>
   <si>
     <t>Stable</t>
+  </si>
+  <si>
+    <t>16.569 J of energy</t>
+  </si>
+  <si>
+    <t>Did some extra venting, looks like gas purity is very important!</t>
   </si>
 </sst>
 </file>
@@ -1022,9 +1029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51ACE552-DDB5-43E8-AB25-900D2EB1BA03}">
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M22" sqref="M22"/>
+      <selection pane="topRight" activeCell="P76" sqref="P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4907,6 +4914,9 @@
       <c r="S67" t="s">
         <v>33</v>
       </c>
+      <c r="T67" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68">
@@ -5025,64 +5035,224 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
       <c r="C70">
         <f>COUNTIF(B$2:B70, B70)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D70" t="str">
         <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP69_0</v>
-      </c>
-      <c r="F70" s="4"/>
-      <c r="K70" s="5"/>
+        <v>LSP69_X9</v>
+      </c>
+      <c r="E70" s="1">
+        <v>45152</v>
+      </c>
+      <c r="F70" s="4">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G70" t="s">
+        <v>13</v>
+      </c>
+      <c r="H70">
+        <v>16.155000000000001</v>
+      </c>
+      <c r="I70" t="s">
+        <v>52</v>
+      </c>
+      <c r="J70" t="s">
+        <v>14</v>
+      </c>
+      <c r="K70" s="5">
+        <v>10.35</v>
+      </c>
+      <c r="L70">
+        <v>201</v>
+      </c>
+      <c r="M70" t="s">
+        <v>45</v>
+      </c>
+      <c r="N70" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q70">
+        <v>1262</v>
+      </c>
+      <c r="R70">
+        <v>8</v>
+      </c>
+      <c r="S70" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
+      <c r="B71" t="s">
+        <v>71</v>
+      </c>
       <c r="C71">
         <f>COUNTIF(B$2:B71, B71)</f>
+        <v>10</v>
+      </c>
+      <c r="D71" t="str">
+        <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
+        <v>LSP70_X10</v>
+      </c>
+      <c r="E71" s="1">
+        <v>45152</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H71">
+        <v>15</v>
+      </c>
+      <c r="I71" t="s">
+        <v>76</v>
+      </c>
+      <c r="J71" t="s">
+        <v>14</v>
+      </c>
+      <c r="K71" s="5">
+        <v>10.35</v>
+      </c>
+      <c r="L71">
+        <v>202</v>
+      </c>
+      <c r="M71" t="s">
+        <v>45</v>
+      </c>
+      <c r="N71" t="b">
         <v>0</v>
       </c>
-      <c r="D71" t="str">
-        <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP70_0</v>
-      </c>
-      <c r="F71" s="4"/>
-      <c r="K71" s="5"/>
+      <c r="Q71">
+        <v>1266</v>
+      </c>
+      <c r="R71">
+        <v>8</v>
+      </c>
+      <c r="S71" t="s">
+        <v>33</v>
+      </c>
+      <c r="T71" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
       <c r="C72">
         <f>COUNTIF(B$2:B72, B72)</f>
+        <v>11</v>
+      </c>
+      <c r="D72" t="str">
+        <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
+        <v>LSP71_X11</v>
+      </c>
+      <c r="E72" s="1">
+        <v>45152</v>
+      </c>
+      <c r="F72" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H72">
+        <v>15</v>
+      </c>
+      <c r="I72" t="s">
+        <v>49</v>
+      </c>
+      <c r="J72" t="s">
+        <v>14</v>
+      </c>
+      <c r="K72" s="5">
+        <v>10.34</v>
+      </c>
+      <c r="L72">
+        <v>203</v>
+      </c>
+      <c r="M72" t="s">
+        <v>45</v>
+      </c>
+      <c r="N72" t="b">
         <v>0</v>
       </c>
-      <c r="D72" t="str">
-        <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP71_0</v>
-      </c>
-      <c r="F72" s="4"/>
-      <c r="K72" s="5"/>
+      <c r="Q72">
+        <v>1268</v>
+      </c>
+      <c r="R72">
+        <v>8</v>
+      </c>
+      <c r="S72" t="s">
+        <v>33</v>
+      </c>
+      <c r="T72" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
+      <c r="B73" t="s">
+        <v>71</v>
+      </c>
       <c r="C73">
         <f>COUNTIF(B$2:B73, B73)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D73" t="str">
         <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP72_0</v>
-      </c>
-      <c r="F73" s="4"/>
-      <c r="K73" s="5"/>
+        <v>LSP72_X12</v>
+      </c>
+      <c r="E73" s="1">
+        <v>45152</v>
+      </c>
+      <c r="F73" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H73">
+        <v>15</v>
+      </c>
+      <c r="I73" t="s">
+        <v>49</v>
+      </c>
+      <c r="J73" t="s">
+        <v>14</v>
+      </c>
+      <c r="K73" s="5">
+        <v>10.37</v>
+      </c>
+      <c r="L73">
+        <v>204</v>
+      </c>
+      <c r="M73" t="s">
+        <v>45</v>
+      </c>
+      <c r="N73" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q73">
+        <v>12610</v>
+      </c>
+      <c r="R73">
+        <v>8</v>
+      </c>
+      <c r="S73" t="s">
+        <v>33</v>
+      </c>
+      <c r="T73" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74">

</xml_diff>

<commit_message>
much writing very wow
</commit_message>
<xml_diff>
--- a/rawdata/shotlist_Aug9.xlsx
+++ b/rawdata/shotlist_Aug9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Repositories\MScThesis\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5BF328-554D-4C67-A7DD-195BF991CE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738843BA-2145-4D26-A425-CF52B4DFD2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{52462B7A-835B-47F1-ADEF-6175C6EA22AF}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{52462B7A-835B-47F1-ADEF-6175C6EA22AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Shotlist V2" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Information" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="109">
   <si>
     <t>Shot #</t>
   </si>
@@ -398,6 +397,18 @@
   </si>
   <si>
     <t>Did some extra venting, looks like gas purity is very important!</t>
+  </si>
+  <si>
+    <t>Nozzle Diameter [mm]</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Troubleshooting spectrometry fiber</t>
+  </si>
+  <si>
+    <t>Troubleshooting spectrometry fiber - fixed. Use 100 micron fiber for targeting</t>
   </si>
 </sst>
 </file>
@@ -660,9 +671,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{775A9C91-55BB-4E85-B6A8-04F894FBEA7D}" name="Shotlist4" displayName="Shotlist4" ref="A1:T100" totalsRowShown="0">
-  <autoFilter ref="A1:T100" xr:uid="{FE804A28-01CE-4180-9E8F-A6762557ED61}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{775A9C91-55BB-4E85-B6A8-04F894FBEA7D}" name="Shotlist4" displayName="Shotlist4" ref="A1:U100" totalsRowShown="0">
+  <autoFilter ref="A1:U100" xr:uid="{FE804A28-01CE-4180-9E8F-A6762557ED61}"/>
+  <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{AEDB9902-D3F1-4EB8-96BB-33DA3A944DF4}" name="Index" dataDxfId="8">
       <calculatedColumnFormula>IF(ISNUMBER(A1), A1+1, 1)</calculatedColumnFormula>
     </tableColumn>
@@ -688,6 +699,7 @@
     <tableColumn id="11" xr3:uid="{F50626E1-104C-48C3-97D9-5E133B21B031}" name="Oscilloscope Data"/>
     <tableColumn id="15" xr3:uid="{179065F3-5426-4679-A28A-A4503F50FCF7}" name="Aperture"/>
     <tableColumn id="13" xr3:uid="{15FF45C8-3CA3-4457-947C-FF42785F6279}" name="ND"/>
+    <tableColumn id="21" xr3:uid="{61810D49-3D0B-4A8D-8239-E35C20D1E7FA}" name="Nozzle Diameter [mm]"/>
     <tableColumn id="12" xr3:uid="{08E34779-25BD-441E-89BE-669E6F0A4DC8}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1027,35 +1039,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51ACE552-DDB5-43E8-AB25-900D2EB1BA03}">
-  <dimension ref="A1:V100"/>
+  <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P76" sqref="P76"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L73" sqref="L73:L78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.53515625" customWidth="1"/>
+    <col min="2" max="2" width="14.3046875" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="13.3828125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.69140625" customWidth="1"/>
+    <col min="7" max="7" width="8.3828125" customWidth="1"/>
     <col min="8" max="9" width="18" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" customWidth="1"/>
-    <col min="17" max="17" width="35.7109375" customWidth="1"/>
-    <col min="18" max="19" width="16.5703125" customWidth="1"/>
-    <col min="20" max="20" width="80.42578125" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.53515625" customWidth="1"/>
+    <col min="12" max="13" width="19.3828125" customWidth="1"/>
+    <col min="14" max="14" width="10.69140625" customWidth="1"/>
+    <col min="15" max="15" width="24.84375" customWidth="1"/>
+    <col min="16" max="16" width="18.3828125" customWidth="1"/>
+    <col min="17" max="17" width="35.69140625" customWidth="1"/>
+    <col min="18" max="19" width="16.53515625" customWidth="1"/>
+    <col min="20" max="20" width="21.69140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="76.3828125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1114,13 +1127,16 @@
         <v>31</v>
       </c>
       <c r="T1" t="s">
+        <v>105</v>
+      </c>
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2">
         <f t="shared" ref="A2:A51" si="0">IF(ISNUMBER(A1), A1+1, 1)</f>
         <v>1</v>
@@ -1175,14 +1191,14 @@
       <c r="S2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>82</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1234,11 +1250,11 @@
       <c r="S3" t="s">
         <v>33</v>
       </c>
-      <c r="V3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1291,7 +1307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1343,11 +1359,11 @@
       <c r="S5" t="s">
         <v>33</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1399,11 +1415,11 @@
       <c r="S6" t="s">
         <v>33</v>
       </c>
-      <c r="V6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1456,7 +1472,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1508,11 +1524,11 @@
       <c r="S8" t="s">
         <v>33</v>
       </c>
-      <c r="V8" s="3" t="s">
+      <c r="W8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1564,11 +1580,11 @@
       <c r="S9" t="s">
         <v>33</v>
       </c>
-      <c r="V9">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1620,11 +1636,11 @@
       <c r="S10" t="s">
         <v>33</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1679,14 +1695,14 @@
       <c r="S11" t="s">
         <v>33</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>53</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1741,14 +1757,14 @@
       <c r="S12" t="s">
         <v>33</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>54</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1803,11 +1819,11 @@
       <c r="S13" t="s">
         <v>33</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1862,14 +1878,14 @@
       <c r="S14" t="s">
         <v>33</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>58</v>
       </c>
-      <c r="V14" s="3" t="s">
+      <c r="W14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1924,14 +1940,14 @@
       <c r="S15" t="s">
         <v>33</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>60</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>4.3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1986,14 +2002,14 @@
       <c r="S16" t="s">
         <v>33</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>62</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>4.75</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2048,14 +2064,14 @@
       <c r="S17" t="s">
         <v>33</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>63</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2110,14 +2126,14 @@
       <c r="S18" t="s">
         <v>33</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>64</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>9.18</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2172,11 +2188,11 @@
       <c r="S19" t="s">
         <v>33</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2231,14 +2247,14 @@
       <c r="S20" t="s">
         <v>33</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>73</v>
       </c>
-      <c r="V20" s="3" t="s">
+      <c r="W20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2293,14 +2309,14 @@
       <c r="S21" t="s">
         <v>33</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>68</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2355,14 +2371,14 @@
       <c r="S22" t="s">
         <v>33</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>69</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2417,14 +2433,14 @@
       <c r="S23" t="s">
         <v>33</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>75</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2479,14 +2495,14 @@
       <c r="S24" t="s">
         <v>33</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>70</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2538,11 +2554,11 @@
       <c r="S25" t="s">
         <v>33</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2594,11 +2610,11 @@
       <c r="S26" t="s">
         <v>33</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2650,14 +2666,14 @@
       <c r="S27" t="s">
         <v>33</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>72</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2709,11 +2725,11 @@
       <c r="S28" t="s">
         <v>33</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2765,14 +2781,14 @@
       <c r="S29" t="s">
         <v>33</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>72</v>
       </c>
-      <c r="V29" s="3" t="s">
+      <c r="W29" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2824,14 +2840,14 @@
       <c r="S30" t="s">
         <v>33</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>74</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2883,11 +2899,11 @@
       <c r="S31" t="s">
         <v>33</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>5.6</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2939,11 +2955,11 @@
       <c r="S32" t="s">
         <v>33</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2995,11 +3011,11 @@
       <c r="S33" t="s">
         <v>33</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3051,14 +3067,14 @@
       <c r="S34" t="s">
         <v>33</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>72</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3110,11 +3126,11 @@
       <c r="S35" t="s">
         <v>33</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3167,7 +3183,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3219,11 +3235,11 @@
       <c r="S37" t="s">
         <v>33</v>
       </c>
-      <c r="V37" s="3" t="s">
+      <c r="W37" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3275,11 +3291,11 @@
       <c r="S38" t="s">
         <v>33</v>
       </c>
-      <c r="V38" t="s">
+      <c r="W38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3331,11 +3347,11 @@
       <c r="S39" t="s">
         <v>33</v>
       </c>
-      <c r="V39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3387,11 +3403,11 @@
       <c r="S40" t="s">
         <v>33</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3443,14 +3459,14 @@
       <c r="S41" t="s">
         <v>33</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>72</v>
       </c>
-      <c r="V41" s="3" t="s">
+      <c r="W41" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3503,7 +3519,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3555,11 +3571,11 @@
       <c r="S43" t="s">
         <v>33</v>
       </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3612,7 +3628,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3664,11 +3680,11 @@
       <c r="S45" t="s">
         <v>33</v>
       </c>
-      <c r="T45" t="s">
+      <c r="U45" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3721,7 +3737,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3773,11 +3789,11 @@
       <c r="S47" t="s">
         <v>33</v>
       </c>
-      <c r="T47" t="s">
+      <c r="U47" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3829,11 +3845,11 @@
       <c r="S48" t="s">
         <v>33</v>
       </c>
-      <c r="T48" t="s">
+      <c r="U48" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3885,11 +3901,11 @@
       <c r="S49" t="s">
         <v>33</v>
       </c>
-      <c r="T49" t="s">
+      <c r="U49" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3941,11 +3957,11 @@
       <c r="S50" t="s">
         <v>33</v>
       </c>
-      <c r="T50" t="s">
+      <c r="U50" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3997,11 +4013,11 @@
       <c r="S51" t="s">
         <v>33</v>
       </c>
-      <c r="T51" t="s">
+      <c r="U51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A52">
         <f>IF(ISNUMBER(A51), A51+1, 1)</f>
         <v>51</v>
@@ -4057,7 +4073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A53">
         <f t="shared" ref="A53:A100" si="1">IF(ISNUMBER(A52), A52+1, 1)</f>
         <v>52</v>
@@ -4113,7 +4129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -4169,7 +4185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -4225,7 +4241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -4280,11 +4296,11 @@
       <c r="S56" t="s">
         <v>33</v>
       </c>
-      <c r="T56" t="s">
+      <c r="U56" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -4340,7 +4356,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -4395,11 +4411,11 @@
       <c r="S58" t="s">
         <v>33</v>
       </c>
-      <c r="T58" t="s">
+      <c r="U58" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -4451,11 +4467,11 @@
       <c r="S59" t="s">
         <v>33</v>
       </c>
-      <c r="T59" t="s">
+      <c r="U59" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -4507,11 +4523,11 @@
       <c r="S60" t="s">
         <v>33</v>
       </c>
-      <c r="T60" t="s">
+      <c r="U60" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -4566,11 +4582,11 @@
       <c r="S61" t="s">
         <v>33</v>
       </c>
-      <c r="T61" t="s">
+      <c r="U61" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -4625,11 +4641,11 @@
       <c r="S62" t="s">
         <v>33</v>
       </c>
-      <c r="T62" t="s">
+      <c r="U62" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -4684,11 +4700,11 @@
       <c r="S63" t="s">
         <v>33</v>
       </c>
-      <c r="T63" t="s">
+      <c r="U63" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -4744,7 +4760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -4800,7 +4816,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -4855,11 +4871,11 @@
       <c r="S66" t="s">
         <v>33</v>
       </c>
-      <c r="T66" t="s">
+      <c r="U66" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A67">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -4914,11 +4930,11 @@
       <c r="S67" t="s">
         <v>33</v>
       </c>
-      <c r="T67" t="s">
+      <c r="U67" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -4970,11 +4986,11 @@
       <c r="S68" t="s">
         <v>33</v>
       </c>
-      <c r="T68" t="s">
+      <c r="U68" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -5026,11 +5042,11 @@
       <c r="S69" t="s">
         <v>33</v>
       </c>
-      <c r="T69" t="s">
+      <c r="U69" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -5068,7 +5084,7 @@
         <v>10.35</v>
       </c>
       <c r="L70">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M70" t="s">
         <v>45</v>
@@ -5086,7 +5102,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -5108,6 +5124,9 @@
       <c r="F71" s="4">
         <v>0.2</v>
       </c>
+      <c r="G71" t="s">
+        <v>13</v>
+      </c>
       <c r="H71">
         <v>15</v>
       </c>
@@ -5121,7 +5140,7 @@
         <v>10.35</v>
       </c>
       <c r="L71">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M71" t="s">
         <v>45</v>
@@ -5138,11 +5157,11 @@
       <c r="S71" t="s">
         <v>33</v>
       </c>
-      <c r="T71" t="s">
+      <c r="U71" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -5164,6 +5183,9 @@
       <c r="F72" s="4">
         <v>0.2</v>
       </c>
+      <c r="G72" t="s">
+        <v>13</v>
+      </c>
       <c r="H72">
         <v>15</v>
       </c>
@@ -5177,7 +5199,7 @@
         <v>10.34</v>
       </c>
       <c r="L72">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M72" t="s">
         <v>45</v>
@@ -5194,11 +5216,11 @@
       <c r="S72" t="s">
         <v>33</v>
       </c>
-      <c r="T72" t="s">
+      <c r="U72" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -5220,6 +5242,9 @@
       <c r="F73" s="4">
         <v>0.2</v>
       </c>
+      <c r="G73" t="s">
+        <v>13</v>
+      </c>
       <c r="H73">
         <v>15</v>
       </c>
@@ -5233,7 +5258,7 @@
         <v>10.37</v>
       </c>
       <c r="L73">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="M73" t="s">
         <v>45</v>
@@ -5250,91 +5275,291 @@
       <c r="S73" t="s">
         <v>33</v>
       </c>
-      <c r="T73" t="s">
+      <c r="U73" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>106</v>
+      </c>
       <c r="C74">
         <f>COUNTIF(B$2:B74, B74)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" t="str">
         <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP73_0</v>
-      </c>
-      <c r="F74" s="4"/>
-      <c r="K74" s="5"/>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+        <v>LSP73_F1</v>
+      </c>
+      <c r="E74" s="1">
+        <v>45153</v>
+      </c>
+      <c r="F74" s="4">
+        <v>1</v>
+      </c>
+      <c r="G74" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74">
+        <v>10</v>
+      </c>
+      <c r="I74" t="s">
+        <v>52</v>
+      </c>
+      <c r="J74" t="s">
+        <v>14</v>
+      </c>
+      <c r="K74" s="5">
+        <v>9.33</v>
+      </c>
+      <c r="L74">
+        <v>200</v>
+      </c>
+      <c r="M74" t="s">
+        <v>45</v>
+      </c>
+      <c r="N74" t="b">
+        <v>1</v>
+      </c>
+      <c r="R74">
+        <v>22</v>
+      </c>
+      <c r="S74" t="s">
+        <v>33</v>
+      </c>
+      <c r="T74">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
+      <c r="B75" t="s">
+        <v>106</v>
+      </c>
       <c r="C75">
         <f>COUNTIF(B$2:B75, B75)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D75" t="str">
         <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP74_0</v>
-      </c>
-      <c r="F75" s="4"/>
-      <c r="K75" s="5"/>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+        <v>LSP74_F2</v>
+      </c>
+      <c r="E75" s="1">
+        <v>45153</v>
+      </c>
+      <c r="F75" s="4">
+        <v>1</v>
+      </c>
+      <c r="G75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75">
+        <v>10</v>
+      </c>
+      <c r="I75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J75" t="s">
+        <v>14</v>
+      </c>
+      <c r="K75" s="5">
+        <v>10</v>
+      </c>
+      <c r="L75">
+        <v>200</v>
+      </c>
+      <c r="M75" t="s">
+        <v>45</v>
+      </c>
+      <c r="N75" t="b">
+        <v>1</v>
+      </c>
+      <c r="R75">
+        <v>22</v>
+      </c>
+      <c r="S75" t="s">
+        <v>33</v>
+      </c>
+      <c r="T75">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>106</v>
+      </c>
       <c r="C76">
         <f>COUNTIF(B$2:B76, B76)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D76" t="str">
         <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP75_0</v>
-      </c>
-      <c r="F76" s="4"/>
-      <c r="K76" s="5"/>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+        <v>LSP75_F3</v>
+      </c>
+      <c r="E76" s="1">
+        <v>45153</v>
+      </c>
+      <c r="F76" s="4">
+        <v>1</v>
+      </c>
+      <c r="G76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H76">
+        <v>10</v>
+      </c>
+      <c r="I76" t="s">
+        <v>52</v>
+      </c>
+      <c r="J76" t="s">
+        <v>14</v>
+      </c>
+      <c r="K76" s="5">
+        <v>9.9969999999999999</v>
+      </c>
+      <c r="L76">
+        <v>200</v>
+      </c>
+      <c r="M76" t="s">
+        <v>45</v>
+      </c>
+      <c r="N76" t="b">
+        <v>1</v>
+      </c>
+      <c r="R76">
+        <v>22</v>
+      </c>
+      <c r="S76" t="s">
+        <v>33</v>
+      </c>
+      <c r="T76">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
+      <c r="B77" t="s">
+        <v>71</v>
+      </c>
       <c r="C77">
         <f>COUNTIF(B$2:B77, B77)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D77" t="str">
         <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP76_0</v>
-      </c>
-      <c r="F77" s="4"/>
-      <c r="K77" s="5"/>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+        <v>LSP76_X13</v>
+      </c>
+      <c r="E77" s="1">
+        <v>45153</v>
+      </c>
+      <c r="F77" s="4">
+        <v>1</v>
+      </c>
+      <c r="G77" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77">
+        <v>10</v>
+      </c>
+      <c r="I77" t="s">
+        <v>52</v>
+      </c>
+      <c r="J77" t="s">
+        <v>14</v>
+      </c>
+      <c r="K77" s="5">
+        <v>10.01</v>
+      </c>
+      <c r="L77">
+        <v>200</v>
+      </c>
+      <c r="M77" t="s">
+        <v>45</v>
+      </c>
+      <c r="N77" t="b">
+        <v>1</v>
+      </c>
+      <c r="R77">
+        <v>22</v>
+      </c>
+      <c r="S77" t="s">
+        <v>33</v>
+      </c>
+      <c r="U77" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
+      <c r="B78" t="s">
+        <v>71</v>
+      </c>
       <c r="C78">
         <f>COUNTIF(B$2:B78, B78)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D78" t="str">
         <f>"LSP"&amp;Shotlist4[[#This Row],[Index]]&amp;"_"&amp;Shotlist4[[#This Row],[Series Prefix]]&amp;Shotlist4[[#This Row],[Series Index]]</f>
-        <v>LSP77_0</v>
-      </c>
-      <c r="F78" s="4"/>
-      <c r="K78" s="5"/>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+        <v>LSP77_X14</v>
+      </c>
+      <c r="E78" s="1">
+        <v>45153</v>
+      </c>
+      <c r="F78" s="4">
+        <v>1</v>
+      </c>
+      <c r="G78" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78">
+        <v>10</v>
+      </c>
+      <c r="I78" t="s">
+        <v>52</v>
+      </c>
+      <c r="J78" t="s">
+        <v>14</v>
+      </c>
+      <c r="K78" s="5">
+        <v>10.01</v>
+      </c>
+      <c r="L78">
+        <v>200</v>
+      </c>
+      <c r="M78" t="s">
+        <v>45</v>
+      </c>
+      <c r="N78" t="b">
+        <v>1</v>
+      </c>
+      <c r="R78">
+        <v>22</v>
+      </c>
+      <c r="S78" t="s">
+        <v>33</v>
+      </c>
+      <c r="U78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -5350,7 +5575,7 @@
       <c r="F79" s="4"/>
       <c r="K79" s="5"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -5366,7 +5591,7 @@
       <c r="F80" s="4"/>
       <c r="K80" s="5"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -5382,7 +5607,7 @@
       <c r="F81" s="4"/>
       <c r="K81" s="5"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -5398,7 +5623,7 @@
       <c r="F82" s="4"/>
       <c r="K82" s="5"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -5414,7 +5639,7 @@
       <c r="F83" s="4"/>
       <c r="K83" s="5"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -5430,7 +5655,7 @@
       <c r="F84" s="4"/>
       <c r="K84" s="5"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -5446,7 +5671,7 @@
       <c r="F85" s="4"/>
       <c r="K85" s="5"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -5462,7 +5687,7 @@
       <c r="F86" s="4"/>
       <c r="K86" s="5"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -5478,7 +5703,7 @@
       <c r="F87" s="4"/>
       <c r="K87" s="5"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -5494,7 +5719,7 @@
       <c r="F88" s="4"/>
       <c r="K88" s="5"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -5510,7 +5735,7 @@
       <c r="F89" s="4"/>
       <c r="K89" s="5"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -5526,7 +5751,7 @@
       <c r="F90" s="4"/>
       <c r="K90" s="5"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -5542,7 +5767,7 @@
       <c r="F91" s="4"/>
       <c r="K91" s="5"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -5558,7 +5783,7 @@
       <c r="F92" s="4"/>
       <c r="K92" s="5"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -5574,7 +5799,7 @@
       <c r="F93" s="4"/>
       <c r="K93" s="5"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -5590,7 +5815,7 @@
       <c r="F94" s="4"/>
       <c r="K94" s="5"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -5606,7 +5831,7 @@
       <c r="F95" s="4"/>
       <c r="K95" s="5"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -5622,7 +5847,7 @@
       <c r="F96" s="4"/>
       <c r="K96" s="5"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -5638,7 +5863,7 @@
       <c r="F97" s="4"/>
       <c r="K97" s="5"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -5654,7 +5879,7 @@
       <c r="F98" s="4"/>
       <c r="K98" s="5"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -5670,7 +5895,7 @@
       <c r="F99" s="4"/>
       <c r="K99" s="5"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -5690,19 +5915,19 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O100" xr:uid="{E9C44812-66A9-47AB-A3E8-CDD9C677A0FE}">
-      <formula1>$V$15:$V$18</formula1>
+      <formula1>$W$15:$W$18</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L100" xr:uid="{1130C877-363F-43B8-87E1-A995FFA14A93}">
-      <formula1>$V$9:$V$12</formula1>
+      <formula1>$W$9:$W$12</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J100" xr:uid="{859F22AC-5CFA-4C4C-8F69-7BCC9C47B468}">
-      <formula1>$V$6</formula1>
+      <formula1>$W$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G100" xr:uid="{821C1184-00AC-4F86-AFC4-797B0848895E}">
-      <formula1>$V$2:$V$3</formula1>
+      <formula1>$W$2:$W$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M100" xr:uid="{1114F14C-0EE3-4BDB-A051-9C6075DA3C72}">
-      <formula1>$V$38:$V$39</formula1>
+      <formula1>$W$38:$W$39</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N100" xr:uid="{C4F2778B-FB48-454D-B6A5-CF5EB7106174}">
       <formula1>"TRUE, FALSE"</formula1>
@@ -5724,24 +5949,24 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.53515625" customWidth="1"/>
+    <col min="2" max="2" width="13.3828125" customWidth="1"/>
+    <col min="3" max="3" width="15.69140625" customWidth="1"/>
+    <col min="4" max="4" width="8.3828125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="35.7109375" customWidth="1"/>
-    <col min="12" max="13" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="75.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" customWidth="1"/>
+    <col min="8" max="8" width="19.3828125" customWidth="1"/>
+    <col min="9" max="9" width="24.84375" customWidth="1"/>
+    <col min="10" max="10" width="18.3828125" customWidth="1"/>
+    <col min="11" max="11" width="35.69140625" customWidth="1"/>
+    <col min="12" max="13" width="16.53515625" customWidth="1"/>
+    <col min="14" max="14" width="75.3828125" customWidth="1"/>
+    <col min="16" max="16" width="9.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5788,7 +6013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2">
         <f t="shared" ref="A2:A30" si="0">IF(ISNUMBER(A1), A1+1, 1)</f>
         <v>1</v>
@@ -5827,7 +6052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -5866,7 +6091,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5902,7 +6127,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5938,7 +6163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5974,7 +6199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6007,7 +6232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6043,7 +6268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6079,7 +6304,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6115,7 +6340,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6151,7 +6376,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6161,7 +6386,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6203,7 +6428,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6248,7 +6473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -6293,7 +6518,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -6338,7 +6563,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6380,7 +6605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6425,7 +6650,7 @@
         <v>9.18</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6467,7 +6692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6512,7 +6737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6554,7 +6779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -6599,7 +6824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -6609,7 +6834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -6619,7 +6844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6629,7 +6854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6639,7 +6864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6649,14 +6874,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6666,7 +6891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6676,7 +6901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31">
         <f t="shared" ref="A31:A37" si="1">IF(ISNUMBER(A30), A30+1, 1)</f>
         <v>30</v>
@@ -6686,7 +6911,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -6696,7 +6921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -6706,7 +6931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -6716,7 +6941,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -6726,112 +6951,112 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38">
         <f t="shared" ref="A38:A51" si="2">IF(ISNUMBER(A37), A37+1, 1)</f>
         <v>37</v>
       </c>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A41">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -6864,19 +7089,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615AE160-9EA4-4070-A5E0-AAC5188A0348}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="69.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" customWidth="1"/>
+    <col min="2" max="2" width="69.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -6884,7 +7109,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -6892,7 +7117,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -6900,12 +7125,17 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>